<commit_message>
Update: sync with improved local project (robust error handling, recovery, real-time monitoring, logging)
</commit_message>
<xml_diff>
--- a/logs/trade_history.xlsx
+++ b/logs/trade_history.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,210 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Entry DateTime</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Index</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Direction</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Entry Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Exit DateTime</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Exit Price</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Stop Loss</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Target</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Trailing SL</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Brokerage</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>P&amp;L</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Margin Required</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>% Gain/Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-07-07 09:34:34</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2571025500CE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>119.4</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-07-07 10:04:36</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>107.15</v>
+      </c>
+      <c r="H2" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>167.2</v>
+      </c>
+      <c r="J2" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>75</v>
+      </c>
+      <c r="L2" t="n">
+        <v>41.79</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-918.75</v>
+      </c>
+      <c r="N2" t="n">
+        <v>8955</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>-10.26%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-07-08 12:34:00</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2571025500CE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>84.59999999999999</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-08 13:04:03</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="H3" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="I3" t="n">
+        <v>118.4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>75</v>
+      </c>
+      <c r="L3" t="n">
+        <v>41.27</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-378.75</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6345</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>-5.97%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit: Add finalized Nifty options strategy with robust trade logging, brokerage, margin, and P&L calculations
</commit_message>
<xml_diff>
--- a/logs/trade_history.xlsx
+++ b/logs/trade_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,6 +628,649 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-07-22 09:42:12</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425100PE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>79.2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-22 09:47:16</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>110.8</v>
+      </c>
+      <c r="J4" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>75</v>
+      </c>
+      <c r="L4" t="n">
+        <v>41.19</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1252.5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>5940</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>-21.09%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-07-22 09:55:54</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425100PE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>72.90000000000001</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-22 10:06:27</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>75.05</v>
+      </c>
+      <c r="H5" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>102.1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="K5" t="n">
+        <v>75</v>
+      </c>
+      <c r="L5" t="n">
+        <v>41.09</v>
+      </c>
+      <c r="M5" t="n">
+        <v>113.9499999999994</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5467.5</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2.95%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-07-23 09:32:20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425150PE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>80.8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-07-23 09:49:46</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>85.59999999999999</v>
+      </c>
+      <c r="H6" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>113.2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="K6" t="n">
+        <v>75</v>
+      </c>
+      <c r="L6" t="n">
+        <v>41.21</v>
+      </c>
+      <c r="M6" t="n">
+        <v>360</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6060</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>5.94%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:03:25</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425100PE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-23 nan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="I7" t="n">
+        <v>80</v>
+      </c>
+      <c r="J7" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="K7" t="n">
+        <v>75</v>
+      </c>
+      <c r="L7" t="n">
+        <v>40.86</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>4290</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:45:07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425100CE</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>73.55</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-07-23 11:12:07</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>81.7</v>
+      </c>
+      <c r="H8" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="I8" t="n">
+        <v>103</v>
+      </c>
+      <c r="J8" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>75</v>
+      </c>
+      <c r="L8" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>611.25</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5516.25</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>11.08%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-07-23 11:57:52</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425100CE</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>84</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-07-23 12:12:52</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>93.59999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>117.6</v>
+      </c>
+      <c r="J9" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="K9" t="n">
+        <v>75</v>
+      </c>
+      <c r="L9" t="n">
+        <v>41.26</v>
+      </c>
+      <c r="M9" t="n">
+        <v>720</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6300</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>11.43%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-07-23 12:37:38</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425150CE</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>79.95</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-07-23 13:07:45</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="H10" t="n">
+        <v>64</v>
+      </c>
+      <c r="I10" t="n">
+        <v>111.8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>64</v>
+      </c>
+      <c r="K10" t="n">
+        <v>75</v>
+      </c>
+      <c r="L10" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-525</v>
+      </c>
+      <c r="N10" t="n">
+        <v>5996.25</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>-8.76%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-07-23 13:22:51</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY2572425200PE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-07-23 13:52:40</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="H11" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>100.1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="K11" t="n">
+        <v>75</v>
+      </c>
+      <c r="L11" t="n">
+        <v>41.07</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-1110</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5362.5</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>-20.70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-07-24 11:15:04</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY25JUL25000PE</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-07-24 11:29:22</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>71.25</v>
+      </c>
+      <c r="H12" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>86</v>
+      </c>
+      <c r="J12" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>75</v>
+      </c>
+      <c r="L12" t="n">
+        <v>40.92</v>
+      </c>
+      <c r="M12" t="n">
+        <v>738.75</v>
+      </c>
+      <c r="N12" t="n">
+        <v>4605</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>16.04%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-07-24 13:00:06</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY25JUL25000PE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>102.45</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-07-24 nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>82</v>
+      </c>
+      <c r="I13" t="n">
+        <v>143.4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>82</v>
+      </c>
+      <c r="K13" t="n">
+        <v>75</v>
+      </c>
+      <c r="L13" t="n">
+        <v>41.54</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>7683.75</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-07-25 09:38:24</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NSE:NIFTY25JUL25000PE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>172.65</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>138.1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>241.8</v>
+      </c>
+      <c r="J14" t="n">
+        <v>138.1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>75</v>
+      </c>
+      <c r="L14" t="n">
+        <v>42.59</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>12948.75</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>